<commit_message>
docs: modelo de diseño
</commit_message>
<xml_diff>
--- a/Etapa Construcción - Iteración 1/Riesgos Fase Construcción, Iteración 1 - Anexo I - Kairos - NexTech.xlsx
+++ b/Etapa Construcción - Iteración 1/Riesgos Fase Construcción, Iteración 1 - Anexo I - Kairos - NexTech.xlsx
@@ -693,11 +693,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="362576379"/>
-        <c:axId val="2010038191"/>
+        <c:axId val="1020946738"/>
+        <c:axId val="34398904"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="362576379"/>
+        <c:axId val="1020946738"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -749,10 +749,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2010038191"/>
+        <c:crossAx val="34398904"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2010038191"/>
+        <c:axId val="34398904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -827,7 +827,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362576379"/>
+        <c:crossAx val="1020946738"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>

</xml_diff>